<commit_message>
yeni dil ve kelimeler
</commit_message>
<xml_diff>
--- a/localization/Localization.xlsx
+++ b/localization/Localization.xlsx
@@ -393,20 +393,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18.42578125" customWidth="1" min="1" max="1"/>
     <col width="32.140625" customWidth="1" min="2" max="2"/>
-    <col width="24.7109375" customWidth="1" min="3" max="3"/>
+    <col width="37.28515625" customWidth="1" min="3" max="3"/>
     <col width="41.42578125" customWidth="1" min="4" max="4"/>
     <col width="49.85546875" customWidth="1" min="5" max="5"/>
-    <col width="75.5703125" customWidth="1" min="6" max="6"/>
+    <col width="38.28515625" customWidth="1" min="6" max="6"/>
+    <col width="39.140625" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -440,6 +441,11 @@
           <t>Ru</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Pt</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,6 +478,11 @@
           <t>Настройки</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Definições</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -491,17 +502,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Terminé !</t>
+          <t>Complétez !</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Abgeschlossen!</t>
+          <t>Vollständig!</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Завершено!</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Completo!</t>
         </is>
       </c>
     </row>
@@ -523,7 +539,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Connexion en cours…</t>
+          <t>Connexion...</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -534,6 +550,11 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>Подключение...</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ligar...</t>
         </is>
       </c>
     </row>
@@ -560,12 +581,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Wird geladen...</t>
+          <t>Laden...</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Загрузка...</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Carregando...</t>
         </is>
       </c>
     </row>
@@ -600,6 +626,11 @@
           <t>Играть</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Jogar</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -624,12 +655,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Fläche</t>
+          <t>Bereich</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Область</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Área</t>
         </is>
       </c>
     </row>
@@ -651,81 +687,96 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Progrès réalisés dans la région</t>
+          <t>Progrès dans le domaine</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Fortschritt im Bereich</t>
+          <t>Bereich Fortschritt</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>Прогресс в области</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Progresso da área</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>frontyard</t>
+          <t>no_thanks</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Front Yard</t>
+          <t>No Thanks</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ön Bahçe</t>
+          <t>Hayır, teşekkürler.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Cour avant</t>
+          <t>Pas de remerciement</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Vorgarten</t>
+          <t>Nein Danke</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Передний двор</t>
+          <t>Нет, спасибо</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Não obrigado</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>place_stairs</t>
+          <t>claim</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Place the stairs!</t>
+          <t>Claim</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Merdivenleri yap!</t>
+          <t>Talep Et</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Placez les escaliers !</t>
+          <t>Réclamation</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Die Treppe aufstellen!</t>
+          <t>Anspruch</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Поставьте лестницу!</t>
+          <t>Заявление</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Reclamação</t>
         </is>
       </c>
     </row>
@@ -752,396 +803,1830 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Mach es!</t>
+          <t>Tu es!</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Сделай это!</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Faça-o!</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>reading_room</t>
+          <t>tap_to_claim</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Reading Room</t>
+          <t>Tap To Claim</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Okuma Odası</t>
+          <t>Tıklayın ve Talep Edin</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Salle de lecture</t>
+          <t>Tapez pour réclamer</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Lesesaal</t>
+          <t>Tippen Sie zum Beantragen</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Читальный зал</t>
+          <t>Нажмите, чтобы заявить о себе</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Toque para reclamar</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>lay_floor</t>
+          <t>quit</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Lay the floor!</t>
+          <t>Quit</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Zemini döşe!</t>
+          <t>Çıkış</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Posez le sol !</t>
+          <t>Démissionner</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Verlegen Sie den Boden!</t>
+          <t>Beenden Sie</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Настелите пол!</t>
+          <t>Увольнение</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Desistir</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>quit</t>
+          <t>hammer_note</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Quit</t>
+          <t>Select a box to open the letters</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Çıkış</t>
+          <t>Harf açmak için bir kutu seç</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Quitter</t>
+          <t>Sélectionnez une boîte pour ouvrir les lettres</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Beenden</t>
+          <t>Wählen Sie ein Feld, um die Buchstaben zu öffnen</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Увольнение</t>
+          <t>Выберите ящик, чтобы открыть письма</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Selecionar uma caixa para abrir as cartas</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>hammer_note</t>
+          <t>level</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Select a box to open the letters</t>
+          <t>Level</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Harf açmak için bir kutu seç</t>
+          <t>Seviye</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sélectionnez une case pour ouvrir les lettres</t>
+          <t>Niveau</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Wählen Sie ein Feld aus, um die Buchstaben zu öffnen.</t>
+          <t>Ebene</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Выберите ящик, чтобы открыть письма</t>
+          <t>Уровень</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nível</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>level</t>
+          <t>next</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Level</t>
+          <t>Next</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Seviye</t>
+          <t>Sonraki</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Niveau</t>
+          <t>Suivant</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Stufe</t>
+          <t>Weiter</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Уровень</t>
+          <t>Следующий</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Seguinte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>next</t>
+          <t>previous</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Next</t>
+          <t>Previous</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sonraki</t>
+          <t>Önceki</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Suivant</t>
+          <t>Précédent</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Nächste</t>
+          <t>Vorherige</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Следующий</t>
+          <t>Предыдущий</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Anterior</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>previous</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Previous</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Önceki</t>
+          <t>Ana Sayfa</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Précédent</t>
+          <t>Accueil</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Zurück</t>
+          <t>Startseite</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Предыдущий</t>
+          <t>Главная</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Início</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>bonus</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Home</t>
+          <t>Bonus</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ana Sayfa</t>
+          <t>Bonus</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Accueil</t>
+          <t>Bonus</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Startseite</t>
+          <t>Bonus</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Главная</t>
+          <t>Бонус</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Bónus</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>bonus</t>
+          <t>bedroom</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Bonus</t>
+          <t>Bedroom</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bonus</t>
+          <t>Yatak Odası</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Bonus</t>
+          <t>Chambre à coucher</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Bonus</t>
+          <t>Schlafzimmer</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Бонус</t>
+          <t>Спальня</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Quarto de dormir</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>tap_to_claim</t>
+          <t>bathroom</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Tap To Claim</t>
+          <t>Bathroom</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tıklayın ve Talep Edin</t>
+          <t>Banyo</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Appuyez pour réclamer</t>
+          <t>Salle de bains</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Zum Einlösen antippen</t>
+          <t>Badezimmer</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Нажмите, чтобы заявить о себе</t>
+          <t>Ванная комната</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Casa de banho</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>claim</t>
+          <t>reading_room</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Claim</t>
+          <t>Reading Room</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Talep Et</t>
+          <t>Okuma Odası</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Réclamation</t>
+          <t>Salle de lecture</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Anspruch</t>
+          <t>Lesesaal</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Претензия</t>
+          <t>Читальный зал</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Sala de leitura</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>no_thanks</t>
+          <t>frontyard</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>No Thanks</t>
+          <t>Front Yard</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Hayır, teşekkürler.</t>
+          <t>Ön Bahçe</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Pas de remerciement</t>
+          <t>Cour avant</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Nein Danke</t>
+          <t>Vorgarten</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Нет, спасибо</t>
+          <t>Передний двор</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Pátio da frente</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>place_stairs</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Place the stairs</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Merdivenleri yap</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Placer l'escalier</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Platzieren Sie die Treppe</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Установите лестницу</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Colocar as escadas</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>boy_room</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Boy Room</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Erkek Çocuk Odası</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Chambre de garçon</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Jungenzimmer</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Комната для мальчика</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Quarto de menino</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>girl_room</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Girl Room</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Kız Çocuk Odası</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Chambre de fille</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Mädchenzimmer</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Комната для девочки</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Quarto de menina</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>kitchen</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Kitchen</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Mutfak</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Cuisine</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Küche</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Кухня</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Cozinha</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>laundry</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Laundry</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Çamaşır Odası</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Blanchisserie</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Wäscherei</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Прачечная</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Lavandaria</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>living_room</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Living Room</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Oturma Odası</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Salle de séjour</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Wohnbereich</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Гостиная</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Sala de estar</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>reading_room</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Reading Room</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Okuma Odası</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Salle de lecture</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Lesesaal</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Читальный зал</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Sala de leitura</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>study_room</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Study Room</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Çalışma Odası</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Salle d'étude</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Arbeitszimmer</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Учебный класс</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Sala de estudo</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>lay_floor</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Lay Floor</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Zemini Döşe</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Plancher de pose</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Boden verlegen</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Укладка пола</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Pavimento</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>install_window</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Install Window</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Pencereyi Tak</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Installer une fenêtre</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Fenster installieren</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Установите окно</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Instalar a janela</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>arrange_furniture</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Arrange Furniture</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Mobilyaları Diz</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Disposer des meubles</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Möbel arrangieren</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Расставьте мебель</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Organizar o mobiliário</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>add_bathtub</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Add Bathtub</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Küvet Ekle</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Ajouter une baignoire</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Badewanne hinzufügen</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Добавить ванну</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Adicionar banheira</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>add_decoration</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Add Decoration</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Dekorasyon Ekle</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Ajouter une décoration</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Dekoration hinzufügen</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Добавить украшение</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Adicionar decoração</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>place_bed</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Place Bed</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Yatağı Yerleştir</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Lit d'appoint</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Ort Bett</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Место Кровать</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Local Cama</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>hang_paintings</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Hang Paintings</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Tabloları As</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Accrocher les peintures</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Gemälde aufhängen</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Повесьте картины</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Pendurar quadros</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>place_pet_food</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Place Pet Food</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Pet Maması Koy</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Place Pet Food</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Ort Tiernahrung</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Корм для домашних животных</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Place Pet Food</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>place_coffee_table</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Place Coffee Table</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Sehba Koy</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Table basse Place</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Platz Couchtisch</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Кофейный столик</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Mesa de centro Place</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>paint_floor</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Paint Floor</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Zemini Boya</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Peinture au sol</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Boden streichen</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Малярный пол</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Piso pintado</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>build_stairs</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Build Stairs</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Merdiven Yap</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Construire un escalier</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Treppe bauen</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Постройте лестницу</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Construir escadas</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>install_doors_windows</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Install Doors and Windows</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Kapı ve Pencere Tak</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Installer des portes et des fenêtres</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Türen und Fenster einbauen</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Установка дверей и окон</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Instalar portas e janelas</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>arrange_floor</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Arrange Floor</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Zemini Düzenle</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Disposer de l'étage</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Boden arrangieren</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Устроить пол</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Dispor o pavimento</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>place_plants</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Place Plants</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Bitkileri Yerleştir</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Placer les plantes</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Ort Pflanzen</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Разместить растения</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Colocar plantas</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>place_bookshelf</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Place Bookshelf</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Kitaplığı Koy</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Place Bookshelf</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Platz Bücherregal</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Книжная полка</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Estante Place</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>place_toys</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Place Toys</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Oyuncakları Yerleştir</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Place Toys</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Platz Spielzeug</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Место для игрушек</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Local Brinquedos</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>arrange_books</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Arrange Books</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Kitapları Diz</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Classer les livres</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Bücher ordnen</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Упорядочить книги</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Organizar livros</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>scatter_clouds</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Scatter Clouds</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Bulutları Serp</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Disperser les nuages</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Streuwolken</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Разбросанные облака</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Dispersão de nuvens</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>scatter_stars</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Scatter Stars</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Yıldızları Serp</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Étoiles de dispersion</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Sterne verstreuen</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Разбросанные звезды</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Estrelas de dispersão</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>build_kitchen_counter</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Build Kitchen Counter</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Tezgahı Yap</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Construire un comptoir de cuisine</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Küchentheke bauen</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Построить кухонную стойку</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Construir balcão de cozinha</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>place_fridge</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Place Fridge</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Buzdolabını Yerleştir</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Placez le réfrigérateur</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Platz Kühlschrank</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Место для холодильника</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Colocar o frigorífico</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>arrange_plates</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Arrange Plates</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Tabakları Diz</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Disposer les assiettes</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Teller anordnen</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Разложить тарелки</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Dispor os pratos</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>place_washing_machine</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Place Washing Machine</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Yıkama Makinesini Yerleştir</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Place Machine à laver</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Platz Waschmaschine</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Место Стиральная машина</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Local Máquina de lavar roupa</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>place_dryer</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Place Dryer</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Kurutma Makinesini Yerleştir</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Place Dryer</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Ort Trockner</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Сушилка для белья</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Local Secador</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>place_shelves</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Place Shelves</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Rafları Yerleştir</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Placer des étagères</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Regale platzieren</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Поместите полки</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Colocar prateleiras</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>place_coat_racks</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Place Coat Racks</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Askılıkları Koy</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Placez les porte-manteaux</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Garderobenständer platzieren</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Разместите вешалки для одежды</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Colocar cabides</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>place_ironing_board</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Place Ironing Board</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Ütü Masasını Koy</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Placez la table à repasser</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Platz Bügelbrett</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Поместите гладильную доску</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Colocar a tábua de engomar</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>place_sofas</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Place Sofas</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Koltukları Yerleştir</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Place Sofas</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Platz Sofas</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Место диванов</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Sofás Place</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>place_desk</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Place Desk</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Çalışma Masasını Yerleştir</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Place Desk</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Platz Schreibtisch</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Стол</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Local de trabalho</t>
         </is>
       </c>
     </row>

</xml_diff>